<commit_message>
color coded clue layout
</commit_message>
<xml_diff>
--- a/SNAZ_ClueLayout.xlsx
+++ b/SNAZ_ClueLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI 306\Clue\Clue Layout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Bullshit\ClueGameSNAZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="31">
   <si>
     <t>W</t>
   </si>
@@ -96,6 +96,27 @@
   </si>
   <si>
     <t>SL</t>
+  </si>
+  <si>
+    <t>Number of doors: 13</t>
+  </si>
+  <si>
+    <t>White: door direction tests (in BoardInitTests)</t>
+  </si>
+  <si>
+    <t>Orange: adjacency list tests, inside room</t>
+  </si>
+  <si>
+    <t>Purple: adjacency list tests, room exits</t>
+  </si>
+  <si>
+    <t>Green: adjacency lists beside room entrance</t>
+  </si>
+  <si>
+    <t>Light Purple: walkway scenarios</t>
+  </si>
+  <si>
+    <t>Light Blue: test targets</t>
   </si>
 </sst>
 </file>
@@ -111,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +169,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -161,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -171,12 +222,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -451,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +527,7 @@
     <col min="11" max="23" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="6">
         <v>0</v>
@@ -531,7 +594,7 @@
       </c>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -571,7 +634,7 @@
       <c r="M2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="O2" s="2" t="s">
@@ -602,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -673,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -686,7 +749,7 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -710,7 +773,7 @@
       <c r="L4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="12" t="s">
         <v>20</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -744,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -815,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -861,7 +924,7 @@
       <c r="O6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="10" t="s">
         <v>0</v>
       </c>
       <c r="Q6" s="4" t="s">
@@ -886,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -902,7 +965,7 @@
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="12" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -917,7 +980,7 @@
       <c r="J7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="10" t="s">
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -957,11 +1020,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1021,14 +1084,14 @@
       <c r="U8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="12" t="s">
         <v>0</v>
       </c>
       <c r="W8" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1053,7 +1116,7 @@
       <c r="H9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -1080,7 +1143,7 @@
       <c r="Q9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="10" t="s">
         <v>0</v>
       </c>
       <c r="S9" s="1" t="s">
@@ -1099,7 +1162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1170,7 +1233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1183,7 +1246,7 @@
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1241,7 +1304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1312,7 +1375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1383,7 +1446,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1435,7 +1498,7 @@
       <c r="Q14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="11" t="s">
         <v>23</v>
       </c>
       <c r="S14" s="2" t="s">
@@ -1454,7 +1517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1464,7 +1527,7 @@
       <c r="C15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="12" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1476,7 +1539,7 @@
       <c r="G15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1500,7 +1563,7 @@
       <c r="O15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="P15" s="12" t="s">
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="s">
@@ -1525,7 +1588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1595,8 +1658,9 @@
       <c r="W16" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y16" s="13"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1624,7 +1688,7 @@
       <c r="I17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -1636,7 +1700,7 @@
       <c r="M17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="N17" s="8" t="s">
         <v>0</v>
       </c>
       <c r="O17" s="2" t="s">
@@ -1660,14 +1724,14 @@
       <c r="U17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="V17" s="8" t="s">
         <v>0</v>
       </c>
       <c r="W17" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1725,7 +1789,7 @@
       <c r="S18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="T18" s="12" t="s">
         <v>0</v>
       </c>
       <c r="U18" s="1" t="s">
@@ -1737,8 +1801,9 @@
       <c r="W18" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y18" s="7"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1754,7 +1819,7 @@
       <c r="E19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="10" t="s">
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1784,7 +1849,7 @@
       <c r="O19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="P19" s="12" t="s">
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="s">
@@ -1809,7 +1874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1880,7 +1945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1951,7 +2016,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2000,7 +2065,7 @@
       <c r="P22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" s="8" t="s">
         <v>0</v>
       </c>
       <c r="R22" s="2" t="s">
@@ -2022,7 +2087,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3">
         <v>0</v>
@@ -2088,6 +2153,41 @@
         <v>20</v>
       </c>
       <c r="W23" s="3"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added legend to layout
</commit_message>
<xml_diff>
--- a/SNAZ_ClueLayout.xlsx
+++ b/SNAZ_ClueLayout.xlsx
@@ -132,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +199,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -226,9 +232,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +533,7 @@
     <col min="11" max="23" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="6">
         <v>0</v>
@@ -594,7 +600,7 @@
       </c>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -665,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -736,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -749,7 +755,7 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -773,7 +779,7 @@
       <c r="L4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="11" t="s">
         <v>20</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -807,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -878,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -949,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -965,7 +971,7 @@
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1020,7 +1026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1084,14 +1090,14 @@
       <c r="U8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V8" s="12" t="s">
+      <c r="V8" s="11" t="s">
         <v>0</v>
       </c>
       <c r="W8" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1161,8 +1167,9 @@
       <c r="W9" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9" s="7"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1233,7 +1240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1304,7 +1311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1375,7 +1382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1446,7 +1453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1498,7 +1505,7 @@
       <c r="Q14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="R14" s="13" t="s">
         <v>23</v>
       </c>
       <c r="S14" s="2" t="s">
@@ -1517,7 +1524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1527,7 +1534,7 @@
       <c r="C15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1563,7 +1570,7 @@
       <c r="O15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="12" t="s">
+      <c r="P15" s="11" t="s">
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="s">
@@ -1588,7 +1595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1658,7 +1665,7 @@
       <c r="W16" s="3">
         <v>14</v>
       </c>
-      <c r="Y16" s="13"/>
+      <c r="Y16" s="12"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1688,7 +1695,7 @@
       <c r="I17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="11" t="s">
         <v>9</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -1789,7 +1796,7 @@
       <c r="S18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T18" s="12" t="s">
+      <c r="T18" s="11" t="s">
         <v>0</v>
       </c>
       <c r="U18" s="1" t="s">
@@ -1849,7 +1856,7 @@
       <c r="O19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P19" s="12" t="s">
+      <c r="P19" s="11" t="s">
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="s">

</xml_diff>